<commit_message>
Add text and update layout for theme and case study tabs
</commit_message>
<xml_diff>
--- a/data-raw/landing_texts.xlsx
+++ b/data-raw/landing_texts.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neilm\Documents\projects\SEAwise_tool\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43E96FC-1D21-4DEE-82AF-E3E13A3F1893}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AD4536-021F-49F4-A8D3-0DCE34B70C18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9105" xr2:uid="{B3A1738F-4730-4C3D-B31B-830F2610B29E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9105" activeTab="2" xr2:uid="{B3A1738F-4730-4C3D-B31B-830F2610B29E}"/>
   </bookViews>
   <sheets>
     <sheet name="landing_page" sheetId="1" r:id="rId1"/>
+    <sheet name="themes" sheetId="2" r:id="rId2"/>
+    <sheet name="case_studies" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>text</t>
   </si>
@@ -70,18 +72,123 @@
   <si>
     <t>welcome</t>
   </si>
+  <si>
+    <t>Environmental changes can have a profound impact on the welfare and productivity of fish stocks. This means that the amount of fish available in a fishery can vary depending on ecological factors, such as water temperature and nutrient availability. 
+Currently, limited understanding of the effects that ecological changes can have on fisheries makes it difficult to predict their potential long-term impacts. This hinders the ability to identify adaptive and responsive management measures. SEAwise aims to deliver a better understanding of this relationship to improve future management advice.
+To achieve this, we’re setting out to:
+Identify the key environmental factors that control productivity.
+Model and predict the ways in which ecological factors could affect fish productivity.
+Incorporate our understanding of how the environment affects fish productivity, as part of the SEAwise fisheries management advice tool.</t>
+  </si>
+  <si>
+    <t>eco_effects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fisheries are often described as part of a “Social Ecological System” – a complex, interactive system in which people and nature are bound together. SEAwise aims to describe and assess the fisheries Social Ecological System, drawing together an understanding of how society, culture, economics, and governance affect fisheries and vice-versa.
+We are working to achieve this by:
+Identifying fisheries-relevant social and economic indicators – statistics that can be used to predict how factors such as wellbeing and unemployment will change over time.
+Working with the industry to identify and model key drivers of fisher behaviour, such as the effect of different management measures on fishing grounds.
+Evaluating the main social and economic impacts of fisheries, including their carbon footprint.
+Identifying methods of fisheries management that promote the welfare of the marine ecosystem whilst protecting social and economic interests.
+Analysing the impacts of fish consumption on human health.
+Summarising and visualising the social and economic effects of fishing as part of the SEAwise management advice tool. </t>
+  </si>
+  <si>
+    <t>socioeconomic_effects</t>
+  </si>
+  <si>
+    <t>fishery_effects</t>
+  </si>
+  <si>
+    <t>spatial_management</t>
+  </si>
+  <si>
+    <t>mse</t>
+  </si>
+  <si>
+    <t>Fisheries are known to have unintentional effects on habitats and species which are not directly targeted by fishing activity. This can include the accidental capture (bycatch) of potentially sensitive species, as well as the potential disturbance of seafloor habitats.
+SEAwise aims to improve our knowledge of these issues, and identify ways in which different management strategies can lessen their impact. This work will also consider the additional influence of non-fishing-related pressures, such as pollution, climate change, invasive species, and algal blooms. 
+To achieve this, we will:
+Identify the key species and habitats impacted by fishing.
+Evaluate the effects of fishing on key ecosystem indicators, including food webs, marine diversity, seafloor and open-sea habitats, fisheries-related litter, and the bycatch of potentially endangered and threatened species.
+Create an online resource which summarises and visualises the environmental impacts of fishing.</t>
+  </si>
+  <si>
+    <t>Determining the causes and effects of changes in fish distribution is vital for effective fisheries management. A number of human activities and environmental conditions are known to affect the locations of fish at sea, such as pollution, fishing impacts, and habitat type. However, current understanding of these relationships is limited.
+SEAwise aims to establish the reasons for and the effects of changing fish distributions, linking these factors to fisheries productivity (the amount of fish available to catch) and selectivity (which fish end up being caught), as well as determining the economic impacts of such changes.
+To achieve this, we will:
+Review what is currently known about the effects of human activities and environmental conditions on the spatial distribution of fish.
+Identify which factors are causing changes in the distributions and life-cycles of commonly-fished species, and predicting how this will be affected by climate change.
+Adapt models to predict how future spatial management measures may affect fisheries’ geographical distribution, selectivity, and profitability.
+Summarise acquired knowledge of the ways in which shifting fish stocks can impact on productivity and the location of fisheries, as part of an online toolkit.</t>
+  </si>
+  <si>
+    <t>In order to establish the most effective recommendations for future fisheries management, it is essential that we utilise existing knowledge and lessons learned. SEAwise aims to evaluate fisheries management plans across Europe, determining which have achieved Good Environmental Status, are economically successful, and protect the well-being of local fishing communities. This information will then be used to develop well-informed, evidence-based future recommendations.
+Our approach involves:
+Identifying the key environmental, economic and social factors that should be considered when evaluating fisheries management strategies.
+Using the knowledge gained from other SEAwise work themes to improve our ability to predict the future effectiveness of management plans.
+Predicting how different management strategies will affect the environment, the economy, and society.
+Estimating suitable targets and thresholds for environmental indicators (e.g. carbon emissions), based on the evaluation of a range management plans.
+Designing region-specific management plans that benefit the environment, the economy, and society.
+Incorporating our understanding of how fisheries impact the environment, the economy and society, within the SEAwise fisheries management advice tool.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Mediterranean Sea is an intercontinental sea that stretches along the southern coast of the European continent, and encompasses the Ionian and Southern Adriatic Seas – areas of particular focus to this case study. 
+This region of the Mediterranean is characterised by it s high biodiversity and socially important small-scale fisheries. Poorly identified and heavily-fished stocks make the Mediterranean ecosystem sensitive to changing environmental conditions. The area is also known for its low biological productivity, meaning that species have slow rates of growth and reproduction. This further complicates management by hindering the potential recovery of the ecosystem as a whole, and its associated fish stocks.
+This case study will work to improve understanding of how fishing affects Mediterranean Sea ecosystems – assessing seafloor impacts, fisheries-related litter, and the accidental capture of sensitive species. Utilising machine learning, new research will predict how climate change, invasive species, and management measures will interact to affect the region’s environment and fisheries, anticipating changes in carbon emissions, catches, and profitability.
+Collaboration with stakeholders will be integral to evaluating the potential social impacts of management advice on different groups in the region. A key goal of the study will be to assess the feasibility of giving Mediterranean fishers greater autonomy in decision-making, while balancing the diverse needs of small- and large-scale fleets. Stakeholder engagement will be achieved through a number of scoping workshops and feedback from end-users – offering local actors the opportunity to voice their needs and contribute their knowledge. Ultimately, SEAwise aims to advance understanding of the interactions between fisheries, the environment, and coastal communities in this unique region, in order to develop advice for EBFM that remains resilient to future change. </t>
+  </si>
+  <si>
+    <t>med_case</t>
+  </si>
+  <si>
+    <t>baltic_case</t>
+  </si>
+  <si>
+    <t>ww_case</t>
+  </si>
+  <si>
+    <t>The Western waters are a subdivision of the Northeast Atlantic that extend from the west coast of Ireland and Scotland to the Strait of Gibraltar. Ranging from the semi-enclosed Irish Sea to the exposed continental shelves of the Celtic Sea and Bay of Biscay, the region is characterised by its diverse marine environments that play host to a broad range of fish stocks and fisheries. This diversity renders effective management challenging – a situation which is further complicated by potential changes to fishing rights following Brexit, changing environmental conditions, and reduced fish growth and reproduction in the area.
+In this case study, SEAwise will develop innovative modelling approaches, combining them with existing models to deliver an improved understanding of the implications of environmental change on fished species. We will assess how different management measures designed to deal with such changes could impact fisheries and the wider marine ecosystem – predicting their influence on catches, carbon emissions, seafloor impacts, fishing-related litter, and bycatch rates. 
+We will also examine the potential effects of management strategies on stakeholders. To achieve this, we will seek the input of coastal communities and recreational users, alongside large- and small-scale fisheries, via a series of scoping workshops and forums for feedback. By integrating social, ecological, and economic considerations into our predictions, we aim to offer well-informed recommendations for the implementation of Ecosystem-Based Fisheries Management in the Western waters.</t>
+  </si>
+  <si>
+    <t>The Baltic Sea is a near-enclosed area of the North Atlantic, nestled between Scandinavia and mainland Europe, and connected to the North Sea via the Skagerrak and Kattegat straits. The region is characterised by areas of low oxygen concentration, historically high contaminant and nutrient levels, and significant interaction between fisheries and marine mammals. Management structures in the Baltic Sea must be adapted to mitigate these challenges in the context of wider ecosystem interactions, while accounting for the additional complexity presented by invasive species and the unprecedented rate of warming in the area.
+In this case study, SEAwise will examine how commercially-important fish stocks (including cod, herring, and sprat) are impacted by changes in environmental and ecological conditions. New research will draw upon existing modelling approaches to evaluate how such changes could alter the wider environmental impacts derived from fisheries. Work will centre around predicting changes in fisheries’ carbon emissions, fishing-related litter, seafloor impacts, and the accidental capture of marine wildlife. The potential effects of different management strategies on the above impacts will also be tested, including under varying climate scenarios. This will ensure that research outputs, and eventual management advice, are resilient to climate change.
+The Ecosystem-Based Fisheries Management advice that results from this case study will be based on the wants and needs of local stakeholders, as well as its predicted ability to meet fisheries and ecological objectives. As such, SEAwise will seek out stakeholder voices via a series of scoping workshops and the SEAwise Stakeholder Network. This will account for the inherent social value of small- and large-scale fisheries in the Baltic Sea, and will also provide an opportunity to incorporate the Traditional Ecological Knowledge of those who call the region home.</t>
+  </si>
+  <si>
+    <t>gns_case</t>
+  </si>
+  <si>
+    <t>The North Sea is situated between the UK, Norway, and mainland Europe, and is host to a wide variety of habitats and commercially-significant fish species. Fisheries in the North Sea are faced with rapidly rising ocean temperatures, increasing demand for offshore wind developments, and changes to fishing-access due to Brexit. The dynamic policy landscape and environmental challenges currently facing the region mean that management advice must be both resilient and responsive to swift change. 
+The North Sea case study will model the cumulative effects of climate change, offshore wind developments, and changes in access to fish stocks and the fisheries that rely on them. By collaborating with stakeholders, we will examine the social importance of the region’s fisheries, exploring how management advice can balance the interests of various large- and small-scale operations, as well as drawing upon local stakeholders’ experience and knowledge. This will be achieved through a series of scoping workshops across the North Sea region, and through ongoing communications with the SEAwise Stakeholder Network.
+Machine-learning algorithms will be utilised across a range of existing databases, alongside more traditional modelling methods, to predict future changes in fisheries’ carbon footprint, bycatch of sensitive species, fishing-related litter, and seafloor impacts. By drawing together these predictions, SEAwise offers holistic Ecosystem-Based Fisheries Management advice, which considers both the rapid changes that are currently happening in the North Sea, and the potential future impacts of different management strategies on fisheries, society, and the region’s ecosystems.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF210384"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="4"/>
+      <color rgb="FF210384"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,10 +211,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -425,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFAC5F67-39A2-465C-88B9-4321F2EB8BB8}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -485,4 +601,146 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055D557F-35EA-4686-BF45-082A320EB9A3}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="30.73046875" customWidth="1"/>
+    <col min="2" max="2" width="79.53125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="213.75" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="162" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="270" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{815C4F49-50D2-4164-9FCA-37290B885711}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B5:B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="72.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="384.75" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="370.5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="327.75" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B11" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add bslib imports to app_ui.R add homepage fix layouts and update navbar
</commit_message>
<xml_diff>
--- a/data-raw/landing_texts.xlsx
+++ b/data-raw/landing_texts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neilm\Documents\projects\SEAwise_tool\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AD4536-021F-49F4-A8D3-0DCE34B70C18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD100775-637D-40A9-8BBA-B6CFE05F62B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9105" activeTab="2" xr2:uid="{B3A1738F-4730-4C3D-B31B-830F2610B29E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9105" xr2:uid="{B3A1738F-4730-4C3D-B31B-830F2610B29E}"/>
   </bookViews>
   <sheets>
     <sheet name="landing_page" sheetId="1" r:id="rId1"/>
@@ -27,47 +27,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>text</t>
   </si>
   <si>
-    <t>how</t>
-  </si>
-  <si>
     <t>section</t>
   </si>
   <si>
-    <t xml:space="preserve">The SEAwise research focuses on 4 case study regions: Mediterranean, Western Waters, North Sea &amp; Baltic.This app displays results of the SEAwise project relating to environmental impacts on fisheries. 
-SEAwise also produces results relating to: Social and Economic impacts of fisheries, Ecological Impacts of fisheries, Spatial management impacts and Fisheries management strategies. 
-Explore the other dimensions of SEAwise by clicking on the links above or via the landing page. </t>
-  </si>
-  <si>
-    <t>content</t>
-  </si>
-  <si>
     <t>who</t>
   </si>
   <si>
-    <t>SEAwise results were generated by a consortium of over 20 research institutes and funded by grant 101000318 of the Horizon 2020 programme.</t>
-  </si>
-  <si>
     <t>website</t>
-  </si>
-  <si>
-    <t>The SEAwise website contains lots of information and results from the project project, that are less technical in nature.</t>
-  </si>
-  <si>
-    <t>The objective of SEAwise is to provide a fully operational approach for European Ecosystem Based Fisheries Management (EBFM) based on persistent networks and co-designed innovation.
-SEAwise addresses this through four objectives:&lt;br&gt;&lt;br&gt;&lt;ol&gt;
- &lt;li&gt;Build a network of stakeholders, advisory bodies, decision makers and scientists to co-design key priorities and approaches to EBFM and to ensure SEAwise’s continued impact long after the project period. &lt;/li&gt; 
- &lt;li&gt;Assemble a new knowledge base on European fisheries interactions with social and ecological systems that integrates scientist and stakeholder experience based knowledge.  &lt;/li&gt; 
- &lt;li&gt;Develop predictive models of fisheries interactions with social and ecological systems to evaluate, select and implement EBFM strategies across Europe accounting for changes in the environment and use of marine space. &lt;/li&gt; 
- &lt;li&gt;Provide ready-for-uptake advice for EBFM for Mediterranean, western and northern European waters. &lt;/li&gt; &lt;/ol&gt;&lt;br&gt;
-To learn more about the SEAwise project, visit the SEAwise &lt;a href="https://seawiseproject.org/"&gt;website&lt;/a&gt;.</t>
-  </si>
-  <si>
-    <t>Please select a case study region from the map to explore environmental impacts upon fisheries there. Click on the tabs at the top of the page to navigate through the app. &lt;p&gt;</t>
   </si>
   <si>
     <t>welcome</t>
@@ -164,6 +135,59 @@
     <t>The North Sea is situated between the UK, Norway, and mainland Europe, and is host to a wide variety of habitats and commercially-significant fish species. Fisheries in the North Sea are faced with rapidly rising ocean temperatures, increasing demand for offshore wind developments, and changes to fishing-access due to Brexit. The dynamic policy landscape and environmental challenges currently facing the region mean that management advice must be both resilient and responsive to swift change. 
 The North Sea case study will model the cumulative effects of climate change, offshore wind developments, and changes in access to fish stocks and the fisheries that rely on them. By collaborating with stakeholders, we will examine the social importance of the region’s fisheries, exploring how management advice can balance the interests of various large- and small-scale operations, as well as drawing upon local stakeholders’ experience and knowledge. This will be achieved through a series of scoping workshops across the North Sea region, and through ongoing communications with the SEAwise Stakeholder Network.
 Machine-learning algorithms will be utilised across a range of existing databases, alongside more traditional modelling methods, to predict future changes in fisheries’ carbon footprint, bycatch of sensitive species, fishing-related litter, and seafloor impacts. By drawing together these predictions, SEAwise offers holistic Ecosystem-Based Fisheries Management advice, which considers both the rapid changes that are currently happening in the North Sea, and the potential future impacts of different management strategies on fisheries, society, and the region’s ecosystems.</t>
+  </si>
+  <si>
+    <t>objective</t>
+  </si>
+  <si>
+    <t>case_study_regions</t>
+  </si>
+  <si>
+    <t>themes</t>
+  </si>
+  <si>
+    <t>To provide a fully operational approach for European Ecosystem Based Fisheries Management (EBFM) based on persistent networks and co-designed innovation.
+SEAwise addresses this through four objectives:&lt;br&gt;&lt;br&gt;&lt;ol&gt;
+ &lt;li&gt;Build a network of stakeholders, advisory bodies, decision makers and scientists to co-design key priorities and approaches to EBFM and to ensure SEAwise’s continued impact long after the project period. &lt;/li&gt; 
+ &lt;li&gt;Assemble a new knowledge base on European fisheries interactions with social and ecological systems that integrates scientist and stakeholder experience based knowledge.  &lt;/li&gt; 
+ &lt;li&gt;Develop predictive models of fisheries interactions with social and ecological systems to evaluate, select and implement EBFM strategies across Europe accounting for changes in the environment and use of marine space. &lt;/li&gt; 
+ &lt;li&gt;Provide ready-for-uptake advice for EBFM for Mediterranean, western and northern European waters. &lt;/li&gt; &lt;/ol&gt;&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>To provide a fully operational approach for European Ecosystem Based Fisheries Management (EBFM) based on persistent networks and co-designed innovation.
+SEAwise addresses this through four objectives:&lt;br&gt;&lt;br&gt;&lt;ol&gt;
+ &lt;li&gt;Build a network of stakeholders &lt;/li&gt; 
+ &lt;li&gt;Assemble a new knowledge base on European fisheries  &lt;/li&gt; 
+ &lt;li&gt;Collate, Develop and Integrate predictive models &lt;/li&gt; 
+ &lt;li&gt;Provide ready-for-uptake advice for Ecosystem Based Fisheries Management &lt;/li&gt; &lt;/ol&gt;&lt;br&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This application displays some of the key research outputs of the SEAwise project. &lt;br&gt;&lt;br&gt;
+Visit the 'About' Tab to learn more about the background and focus areas of SEAwise, or view 'Results' directly. &lt;br&gt;&lt;br&gt;
+</t>
+  </si>
+  <si>
+    <t>SEAwise results were generated by a consortium of 24 parner institutes. &lt;br&gt;&lt;br&gt;
+ SEAwise has received funding from the European Union's Horizon 2020 research and innovation programme under grant agreement No 101000318</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEAwise identifies 5 main themes:&lt;br&gt;&lt;br&gt;&lt;ul&gt;
+&lt;li&gt;Social and economic effects of, and on, fishing &lt;/li&gt;
+&lt;li&gt;Ecological effects on fisheries&lt;/li&gt;
+&lt;li&gt;Ecological effects of fisheries&lt;/li&gt;
+&lt;li&gt;Spatial management impacts on ecological systems and fisheries&lt;/li&gt;
+&lt;li&gt;Evaluation of fisheries management strategies in an ecosystem context&lt;/li&gt;&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>The SEAwise research focuses on 4 case study regions: &lt;br&gt;&lt;br&gt;&lt;ul&gt;
+&lt;li&gt;Mediterranean&lt;/li&gt;
+&lt;li&gt;Western Waters&lt;/li&gt;
+&lt;li&gt;Greater North Sea&lt;/li&gt;
+&lt;li&gt;Baltic&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>The  &lt;a href="https://seawiseproject.org/"&gt;SEAwise project website&lt;/a&gt; contains additional information about the project.</t>
   </si>
 </sst>
 </file>
@@ -539,67 +563,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFAC5F67-39A2-465C-88B9-4321F2EB8BB8}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="143.59765625" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="143.5703125" customWidth="1"/>
+    <col min="3" max="3" width="85.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="210" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
+      <c r="B7" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -607,62 +645,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055D557F-35EA-4686-BF45-082A320EB9A3}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.73046875" customWidth="1"/>
-    <col min="2" max="2" width="79.53125" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="79.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="213.75" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="213.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="313.5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="315" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="162" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="270" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -674,69 +712,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{815C4F49-50D2-4164-9FCA-37290B885711}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B20" sqref="B5:B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="72.19921875" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="72.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="384.75" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="375" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="390" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="370.5" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integrate Med into app
</commit_message>
<xml_diff>
--- a/data-raw/landing_texts.xlsx
+++ b/data-raw/landing_texts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neilm\Documents\projects\SEAwise_tool\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neilm\Projects\SEAwise_tool\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD100775-637D-40A9-8BBA-B6CFE05F62B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15738E4D-0CC5-4DBE-B19C-8F682811743E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9105" xr2:uid="{B3A1738F-4730-4C3D-B31B-830F2610B29E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{B3A1738F-4730-4C3D-B31B-830F2610B29E}"/>
   </bookViews>
   <sheets>
     <sheet name="landing_page" sheetId="1" r:id="rId1"/>
@@ -162,15 +162,6 @@
  &lt;li&gt;Provide ready-for-uptake advice for Ecosystem Based Fisheries Management &lt;/li&gt; &lt;/ol&gt;&lt;br&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">This application displays some of the key research outputs of the SEAwise project. &lt;br&gt;&lt;br&gt;
-Visit the 'About' Tab to learn more about the background and focus areas of SEAwise, or view 'Results' directly. &lt;br&gt;&lt;br&gt;
-</t>
-  </si>
-  <si>
-    <t>SEAwise results were generated by a consortium of 24 parner institutes. &lt;br&gt;&lt;br&gt;
- SEAwise has received funding from the European Union's Horizon 2020 research and innovation programme under grant agreement No 101000318</t>
-  </si>
-  <si>
     <t xml:space="preserve">SEAwise identifies 5 main themes:&lt;br&gt;&lt;br&gt;&lt;ul&gt;
 &lt;li&gt;Social and economic effects of, and on, fishing &lt;/li&gt;
 &lt;li&gt;Ecological effects on fisheries&lt;/li&gt;
@@ -188,6 +179,13 @@
   </si>
   <si>
     <t>The  &lt;a href="https://seawiseproject.org/"&gt;SEAwise project website&lt;/a&gt; contains additional information about the project.</t>
+  </si>
+  <si>
+    <t>SEAwise results were generated by a consortium of 24 partner institutes. &lt;br&gt;&lt;br&gt;
+ SEAwise has received funding from the European Union's Horizon 2020 research and innovation programme under grant agreement No 101000318</t>
+  </si>
+  <si>
+    <t>Select a region below to learn about fisheries there or learn more about SEAwise in &lt;em&gt;About&lt;/em&gt;.</t>
   </si>
 </sst>
 </file>
@@ -267,9 +265,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -307,7 +305,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -413,7 +411,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -555,7 +553,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -566,7 +564,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,12 +582,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="210" x14ac:dyDescent="0.25">
@@ -608,7 +606,7 @@
         <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="165" x14ac:dyDescent="0.25">
@@ -616,7 +614,7 @@
         <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -624,7 +622,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -632,7 +630,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>